<commit_message>
passing on the latest china case study data files
</commit_message>
<xml_diff>
--- a/heliostrome/jip_project/results/test_results_northeastCHINA.xlsx
+++ b/heliostrome/jip_project/results/test_results_northeastCHINA.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -517,6 +517,11 @@
           <t>Init WC - Value</t>
         </is>
       </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Mulch Percentage</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -574,6 +579,9 @@
           <t>[30.01]</t>
         </is>
       </c>
+      <c r="P2" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -631,6 +639,9 @@
           <t>[30.01]</t>
         </is>
       </c>
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -688,6 +699,9 @@
           <t>[30.01]</t>
         </is>
       </c>
+      <c r="P4" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -745,6 +759,9 @@
           <t>[30.01]</t>
         </is>
       </c>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -802,6 +819,7 @@
           <t>[30.01]</t>
         </is>
       </c>
+      <c r="P6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -859,6 +877,7 @@
           <t>[30.01]</t>
         </is>
       </c>
+      <c r="P7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -937,10 +956,10 @@
         <v>251</v>
       </c>
       <c r="F2" t="n">
-        <v>14.17398169766591</v>
+        <v>14.10100213617318</v>
       </c>
       <c r="G2" t="n">
-        <v>151.2598850610039</v>
+        <v>151.0951812105054</v>
       </c>
     </row>
     <row r="3">
@@ -964,10 +983,10 @@
         <v>616</v>
       </c>
       <c r="F3" t="n">
-        <v>14.30457553090168</v>
+        <v>14.23418594620028</v>
       </c>
       <c r="G3" t="n">
-        <v>130.2603605992372</v>
+        <v>130.0945604754279</v>
       </c>
     </row>
     <row r="4">
@@ -991,10 +1010,10 @@
         <v>981</v>
       </c>
       <c r="F4" t="n">
-        <v>14.10789703038272</v>
+        <v>14.03719031314219</v>
       </c>
       <c r="G4" t="n">
-        <v>151.9922915062926</v>
+        <v>151.8214004330344</v>
       </c>
     </row>
     <row r="5">
@@ -1018,10 +1037,10 @@
         <v>1347</v>
       </c>
       <c r="F5" t="n">
-        <v>14.18220979331418</v>
+        <v>14.11877442901446</v>
       </c>
       <c r="G5" t="n">
-        <v>123.6655511553475</v>
+        <v>123.5659772280879</v>
       </c>
     </row>
     <row r="6">
@@ -1045,10 +1064,10 @@
         <v>251</v>
       </c>
       <c r="F6" t="n">
-        <v>14.17398169766591</v>
+        <v>14.10100213617318</v>
       </c>
       <c r="G6" t="n">
-        <v>170.8047151792224</v>
+        <v>170.9516021206933</v>
       </c>
     </row>
     <row r="7">
@@ -1072,10 +1091,10 @@
         <v>616</v>
       </c>
       <c r="F7" t="n">
-        <v>14.30457553090168</v>
+        <v>14.23418594620028</v>
       </c>
       <c r="G7" t="n">
-        <v>150.0545770031289</v>
+        <v>150.2474955590522</v>
       </c>
     </row>
     <row r="8">
@@ -1099,10 +1118,10 @@
         <v>981</v>
       </c>
       <c r="F8" t="n">
-        <v>14.10789703038272</v>
+        <v>14.03719031314219</v>
       </c>
       <c r="G8" t="n">
-        <v>169.1330952719165</v>
+        <v>169.3095168068735</v>
       </c>
     </row>
     <row r="9">
@@ -1126,10 +1145,10 @@
         <v>1347</v>
       </c>
       <c r="F9" t="n">
-        <v>14.18220979331418</v>
+        <v>14.11877442901446</v>
       </c>
       <c r="G9" t="n">
-        <v>145.5912317627781</v>
+        <v>145.7978117690866</v>
       </c>
     </row>
     <row r="10">
@@ -1153,10 +1172,10 @@
         <v>267</v>
       </c>
       <c r="F10" t="n">
-        <v>14.15209118744616</v>
+        <v>14.07795476857072</v>
       </c>
       <c r="G10" t="n">
-        <v>110.7897022513593</v>
+        <v>110.6977645816525</v>
       </c>
     </row>
     <row r="11">
@@ -1180,10 +1199,10 @@
         <v>632</v>
       </c>
       <c r="F11" t="n">
-        <v>14.11859737863568</v>
+        <v>14.0410104232688</v>
       </c>
       <c r="G11" t="n">
-        <v>130.7705436744614</v>
+        <v>130.7076300337451</v>
       </c>
     </row>
     <row r="12">
@@ -1207,10 +1226,10 @@
         <v>997</v>
       </c>
       <c r="F12" t="n">
-        <v>13.76502684284506</v>
+        <v>13.68943921791649</v>
       </c>
       <c r="G12" t="n">
-        <v>156.4679018704647</v>
+        <v>156.3402366909962</v>
       </c>
     </row>
     <row r="13">
@@ -1234,10 +1253,10 @@
         <v>1363</v>
       </c>
       <c r="F13" t="n">
-        <v>14.23680958115403</v>
+        <v>14.16180684707763</v>
       </c>
       <c r="G13" t="n">
-        <v>136.4295070208339</v>
+        <v>136.2284247894075</v>
       </c>
     </row>
     <row r="14">
@@ -1261,10 +1280,10 @@
         <v>267</v>
       </c>
       <c r="F14" t="n">
-        <v>14.15209118744616</v>
+        <v>14.07795476857072</v>
       </c>
       <c r="G14" t="n">
-        <v>128.3873177627219</v>
+        <v>128.5327378042394</v>
       </c>
     </row>
     <row r="15">
@@ -1288,10 +1307,10 @@
         <v>632</v>
       </c>
       <c r="F15" t="n">
-        <v>14.11859737863568</v>
+        <v>14.0410104232688</v>
       </c>
       <c r="G15" t="n">
-        <v>148.8242877716196</v>
+        <v>148.9820792137356</v>
       </c>
     </row>
     <row r="16">
@@ -1315,10 +1334,10 @@
         <v>997</v>
       </c>
       <c r="F16" t="n">
-        <v>13.76502684284506</v>
+        <v>13.68943921791649</v>
       </c>
       <c r="G16" t="n">
-        <v>174.1759787517644</v>
+        <v>174.3338176221372</v>
       </c>
     </row>
     <row r="17">
@@ -1342,10 +1361,10 @@
         <v>1363</v>
       </c>
       <c r="F17" t="n">
-        <v>14.23680958115403</v>
+        <v>14.16180684707763</v>
       </c>
       <c r="G17" t="n">
-        <v>154.0218254956336</v>
+        <v>154.1923213531544</v>
       </c>
     </row>
     <row r="18">
@@ -1369,7 +1388,7 @@
         <v>251</v>
       </c>
       <c r="F18" t="n">
-        <v>12.80812688082464</v>
+        <v>12.73745382988503</v>
       </c>
       <c r="G18" t="n">
         <v>0</v>
@@ -1396,7 +1415,7 @@
         <v>616</v>
       </c>
       <c r="F19" t="n">
-        <v>14.20693048623959</v>
+        <v>14.13354789304776</v>
       </c>
       <c r="G19" t="n">
         <v>0</v>
@@ -1423,7 +1442,7 @@
         <v>981</v>
       </c>
       <c r="F20" t="n">
-        <v>13.83671734355427</v>
+        <v>13.75115892387944</v>
       </c>
       <c r="G20" t="n">
         <v>0</v>
@@ -1450,7 +1469,7 @@
         <v>1347</v>
       </c>
       <c r="F21" t="n">
-        <v>14.09061648046096</v>
+        <v>14.02588107033506</v>
       </c>
       <c r="G21" t="n">
         <v>0</v>
@@ -1477,7 +1496,7 @@
         <v>251</v>
       </c>
       <c r="F22" t="n">
-        <v>12.24033654832572</v>
+        <v>12.14963626658932</v>
       </c>
       <c r="G22" t="n">
         <v>0</v>
@@ -1504,7 +1523,7 @@
         <v>616</v>
       </c>
       <c r="F23" t="n">
-        <v>13.7063128475466</v>
+        <v>13.6092898675149</v>
       </c>
       <c r="G23" t="n">
         <v>0</v>
@@ -1531,7 +1550,7 @@
         <v>981</v>
       </c>
       <c r="F24" t="n">
-        <v>13.61443907375126</v>
+        <v>13.518169953611</v>
       </c>
       <c r="G24" t="n">
         <v>0</v>
@@ -1558,7 +1577,7 @@
         <v>1347</v>
       </c>
       <c r="F25" t="n">
-        <v>13.8058694166582</v>
+        <v>13.73230864875634</v>
       </c>
       <c r="G25" t="n">
         <v>0</v>

</xml_diff>